<commit_message>
V1.1 Update - Oval Topper Mod Added
The ball topper version of the joystick was out of stock for a while so we created an alternate version
that works with the oval topper version.
The enclosure is the same but the thread for the topper is a M10 not an M6. Therefore, a new topper
nut was designed. This was just created to have an insert for a M10 nut without the catch.

Documentation was updated as well.
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Redwood_Joystick_BOM.xlsx
+++ b/Documentation/Working_Documents/Redwood_Joystick_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 24-08 Ultrastik Enclosure/Redwood-Joystick-Github/Redwood_Joystick/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="613" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{475A51D9-84D3-4759-BB9E-150C32A6A7C3}"/>
+  <xr:revisionPtr revIDLastSave="646" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D50DC322-68CF-435A-994E-B7007BD30ECD}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="180" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>Total filament (g)</t>
   </si>
@@ -152,9 +152,6 @@
     <t>https://www.digikey.ca/en/products/detail/serpac/6005/307599</t>
   </si>
   <si>
-    <t>https://www.ultimarc.com/arcade-controls/joysticks/ultrastik-360-oval-top-clone/</t>
-  </si>
-  <si>
     <t>https://www.homedepot.ca/product/paulin-metric-hex-nut-m6-1-00-10pcs/1001588038</t>
   </si>
   <si>
@@ -309,6 +306,72 @@
   </si>
   <si>
     <t>https://www.homedepot.ca/product/paulin-1-4-20-x-1-inch-hex-head-cap-screw-18-8-stainless-steel-unc/1000142352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ultimarc.com/arcade-controls/joysticks/ultrastik-360-oval-top-clone/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UltraStik 360 Oval Top (analog) </t>
+  </si>
+  <si>
+    <t>https://www.ultimarc.com/arcade-controls/joysticks/ultrastik-360-oval-top-en-2/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the ball topper is out of stock you can use the Oval version.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The topper adapter nut will NOT work with this model, you will have to print the alternate version found in the build files.</t>
+    </r>
+  </si>
+  <si>
+    <t>Redwood-Joystick-Topper-Adapter-OvalTopper-v1.0</t>
+  </si>
+  <si>
+    <t>Metric Hex Nut M10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ALTERNATE: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ONLY</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> IF USING "UltraStik 360 Oval Top"</t>
+    </r>
+  </si>
+  <si>
+    <t>ALTERNATE: ONLY IF USING "UltraStik 360 Oval Top"</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.ca/product/paulin-m10-1-50-class-8-metric-hex-nut-din-934-zinc-plated/1000128523</t>
   </si>
 </sst>
 </file>
@@ -319,7 +382,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +448,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -710,7 +782,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -777,16 +849,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="13" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="4" borderId="6" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="13" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -807,11 +885,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1111,17 +1184,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EE8AD1-7DB5-46E4-9BCF-A08DFBDA7B00}">
-  <dimension ref="A1:AV39"/>
+  <dimension ref="A1:AV43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -1139,24 +1212,24 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
+      <c r="B1" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1188,16 +1261,16 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="I5" s="48">
-        <f>SUM(H19:H24)</f>
+        <f>SUM(H21:H26)</f>
         <v>150.34</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="45">
-        <f>K6+K17</f>
-        <v>93.775750000000016</v>
+        <f>K6+K19</f>
+        <v>94.172750000000022</v>
       </c>
       <c r="L5" s="46">
-        <f>L6+L17</f>
+        <f>L6+L19</f>
         <v>97.078749999999999</v>
       </c>
     </row>
@@ -1217,11 +1290,11 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="49">
-        <f>SUM(K8:K16)</f>
-        <v>89.797000000000011</v>
+        <f>SUM(K8:K18)</f>
+        <v>90.194000000000017</v>
       </c>
       <c r="L6" s="7">
-        <f>SUM(L8:L16)</f>
+        <f>SUM(L8:L17)</f>
         <v>93.1</v>
       </c>
       <c r="M6" s="6"/>
@@ -1267,13 +1340,13 @@
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="67" t="s">
-        <v>62</v>
+      <c r="C8" s="65" t="s">
+        <v>61</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="13" t="s">
@@ -1295,11 +1368,11 @@
       <c r="J8" s="57">
         <v>0.63</v>
       </c>
-      <c r="K8" s="69">
+      <c r="K8" s="66">
         <f>IF(G8&gt;0,J8/H8*G8,0)</f>
         <v>2.52</v>
       </c>
-      <c r="L8" s="69">
+      <c r="L8" s="66">
         <f>I8*J8</f>
         <v>2.52</v>
       </c>
@@ -1310,15 +1383,15 @@
     </row>
     <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="77"/>
+        <v>82</v>
+      </c>
+      <c r="D9" s="67"/>
       <c r="E9" s="13" t="s">
         <v>35</v>
       </c>
@@ -1347,19 +1420,19 @@
         <v>83.65</v>
       </c>
       <c r="M9" s="13"/>
-      <c r="N9" s="58" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="66" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>66</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
@@ -1389,19 +1462,19 @@
         <v>0.27</v>
       </c>
       <c r="M10" s="13"/>
-      <c r="N10" s="63" t="s">
-        <v>57</v>
+      <c r="N10" s="62" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>64</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
@@ -1432,37 +1505,37 @@
         <v>0.17</v>
       </c>
       <c r="M11" s="13"/>
-      <c r="N11" s="63" t="s">
+      <c r="N11" s="62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="76"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="78"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
@@ -1494,20 +1567,20 @@
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="77"/>
+      <c r="C14" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="67"/>
       <c r="E14" s="13" t="s">
         <v>34</v>
       </c>
@@ -1535,21 +1608,21 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M14" s="13"/>
-      <c r="N14" s="63" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="N14" s="62" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="77" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="77"/>
+      <c r="C15" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="67"/>
       <c r="E15" s="13" t="s">
         <v>36</v>
       </c>
@@ -1577,21 +1650,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="M15" s="13"/>
-      <c r="N15" s="63" t="s">
+      <c r="N15" s="62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="69" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="77"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="13" t="s">
         <v>36</v>
       </c>
@@ -1619,186 +1690,186 @@
         <v>0.86</v>
       </c>
       <c r="M16" s="13"/>
-      <c r="N16" s="63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="38" t="s">
+      <c r="N16" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="62"/>
+    </row>
+    <row r="18" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="67"/>
+      <c r="E18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="13">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13">
+        <v>10</v>
+      </c>
+      <c r="I18" s="13">
+        <f>IF(G18&gt;0,CEILING(G18/H18,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="57">
+        <v>3.97</v>
+      </c>
+      <c r="K18" s="57">
+        <f t="shared" ref="K18" si="4">IF(G18&gt;0,J18/H18*G18,0)</f>
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="L18" s="57">
+        <f>I18*J18</f>
+        <v>3.97</v>
+      </c>
+      <c r="M18" s="13"/>
+      <c r="N18" s="62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="10">
-        <f>SUM(I19:I26)</f>
-        <v>159.15</v>
-      </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="9">
-        <f>SUM(K19:K25)</f>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="10">
+        <f>SUM(I21:I30)</f>
+        <v>164.02</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="9">
+        <f>SUM(K21:K27)</f>
         <v>3.9787500000000002</v>
       </c>
-      <c r="L17" s="9">
-        <f>SUM(L19:L25)</f>
+      <c r="L19" s="9">
+        <f>SUM(L21:L27)</f>
         <v>3.9787500000000002</v>
       </c>
-      <c r="M17" s="24"/>
-      <c r="N17" s="26"/>
-    </row>
-    <row r="18" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="10" t="s">
+      <c r="M19" s="24"/>
+      <c r="N19" s="26"/>
+    </row>
+    <row r="20" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="18" t="s">
+      <c r="M20" s="10"/>
+      <c r="N20" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="18" t="s">
+      <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18" t="s">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18">
-        <v>1</v>
-      </c>
-      <c r="H19" s="18">
+      <c r="G21" s="18">
+        <v>1</v>
+      </c>
+      <c r="H21" s="18">
         <v>46.15</v>
       </c>
-      <c r="I19" s="18">
-        <f>G19*H19</f>
+      <c r="I21" s="18">
+        <f>G21*H21</f>
         <v>46.15</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J21" s="19">
         <v>25</v>
       </c>
-      <c r="K19" s="19">
-        <f>IF(G19&gt;0,(J19/1000)*G19*H19,0)</f>
+      <c r="K21" s="19">
+        <f>IF(G21&gt;0,(J21/1000)*G21*H21,0)</f>
         <v>1.1537500000000001</v>
       </c>
-      <c r="L19" s="19">
-        <f>K19</f>
+      <c r="L21" s="19">
+        <f>K21</f>
         <v>1.1537500000000001</v>
       </c>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="14">
-        <v>1</v>
-      </c>
-      <c r="H20" s="14">
-        <v>92.63</v>
-      </c>
-      <c r="I20" s="14">
-        <f t="shared" ref="I20" si="4">G20*H20</f>
-        <v>92.63</v>
-      </c>
-      <c r="J20" s="19">
-        <v>25</v>
-      </c>
-      <c r="K20" s="11">
-        <f t="shared" ref="K20" si="5">IF(G20&gt;0,(J20/1000)*G20*H20,0)</f>
-        <v>2.31575</v>
-      </c>
-      <c r="L20" s="11">
-        <f>K20</f>
-        <v>2.31575</v>
-      </c>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A21" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="73"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>20</v>
@@ -1811,110 +1882,53 @@
         <v>1</v>
       </c>
       <c r="H22" s="14">
-        <v>4.87</v>
+        <v>92.63</v>
       </c>
       <c r="I22" s="14">
-        <f t="shared" ref="I22" si="6">G22*H22</f>
-        <v>4.87</v>
+        <f t="shared" ref="I22" si="5">G22*H22</f>
+        <v>92.63</v>
       </c>
       <c r="J22" s="19">
         <v>25</v>
       </c>
       <c r="K22" s="11">
-        <f>IF(G22&gt;0,(J22/1000)*G22*H22,0)</f>
-        <v>0.12175000000000001</v>
+        <f t="shared" ref="K22" si="6">IF(G22&gt;0,(J22/1000)*G22*H22,0)</f>
+        <v>2.31575</v>
       </c>
       <c r="L22" s="11">
-        <f t="shared" ref="L22" si="7">K22</f>
-        <v>0.12175000000000001</v>
+        <f>K22</f>
+        <v>2.31575</v>
       </c>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
     </row>
-    <row r="23" spans="1:48" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="14">
-        <v>1</v>
-      </c>
-      <c r="H23" s="14">
-        <v>0.34</v>
-      </c>
-      <c r="I23" s="14">
-        <f>G23*H23</f>
-        <v>0.34</v>
-      </c>
-      <c r="J23" s="19">
-        <v>25</v>
-      </c>
-      <c r="K23" s="11">
-        <f t="shared" ref="K23:K25" si="8">IF(G23&gt;0,(J23/1000)*G23*H23,0)</f>
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="L23" s="11">
-        <f t="shared" ref="L23:L25" si="9">K23</f>
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="62"/>
-      <c r="X23" s="62"/>
-      <c r="Y23" s="62"/>
-      <c r="Z23" s="62"/>
-      <c r="AA23" s="62"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="62"/>
-      <c r="AD23" s="62"/>
-      <c r="AE23" s="62"/>
-      <c r="AF23" s="62"/>
-      <c r="AG23" s="62"/>
-      <c r="AH23" s="62"/>
-      <c r="AI23" s="62"/>
-      <c r="AJ23" s="62"/>
-      <c r="AK23" s="62"/>
-      <c r="AL23" s="62"/>
-      <c r="AM23" s="62"/>
-      <c r="AN23" s="62"/>
-      <c r="AO23" s="62"/>
-      <c r="AP23" s="62"/>
-      <c r="AQ23" s="62"/>
-      <c r="AR23" s="62"/>
-      <c r="AS23" s="62"/>
-      <c r="AT23" s="62"/>
-      <c r="AU23" s="62"/>
-      <c r="AV23" s="62"/>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A23" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="75"/>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>77</v>
+      <c r="A24" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="65" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>20</v>
@@ -1923,39 +1937,39 @@
       <c r="F24" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="14">
         <v>1</v>
       </c>
       <c r="H24" s="14">
-        <v>6.35</v>
+        <v>4.87</v>
       </c>
       <c r="I24" s="14">
-        <f>G24*H24</f>
-        <v>6.35</v>
+        <f t="shared" ref="I24" si="7">G24*H24</f>
+        <v>4.87</v>
       </c>
       <c r="J24" s="19">
         <v>25</v>
       </c>
       <c r="K24" s="11">
-        <f t="shared" si="8"/>
-        <v>0.15875</v>
+        <f>IF(G24&gt;0,(J24/1000)*G24*H24,0)</f>
+        <v>0.12175000000000001</v>
       </c>
       <c r="L24" s="11">
-        <f t="shared" si="9"/>
-        <v>0.15875</v>
-      </c>
-      <c r="M24" s="18"/>
+        <f t="shared" ref="L24" si="8">K24</f>
+        <v>0.12175000000000001</v>
+      </c>
+      <c r="M24" s="14"/>
       <c r="N24" s="14"/>
     </row>
-    <row r="25" spans="1:48" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>78</v>
+    <row r="25" spans="1:48" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>20</v>
@@ -1964,332 +1978,528 @@
       <c r="F25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="14">
         <v>1</v>
       </c>
       <c r="H25" s="14">
-        <v>8.81</v>
+        <v>0.34</v>
       </c>
       <c r="I25" s="14">
         <f>G25*H25</f>
-        <v>8.81</v>
+        <v>0.34</v>
       </c>
       <c r="J25" s="19">
         <v>25</v>
       </c>
       <c r="K25" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K25:K26" si="9">IF(G25&gt;0,(J25/1000)*G25*H25,0)</f>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="L25" s="11">
+        <f t="shared" ref="L25:L26" si="10">K25</f>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="18">
+        <v>1</v>
+      </c>
+      <c r="H26" s="14">
+        <v>6.35</v>
+      </c>
+      <c r="I26" s="14">
+        <f>G26*H26</f>
+        <v>6.35</v>
+      </c>
+      <c r="J26" s="19">
+        <v>25</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="9"/>
+        <v>0.15875</v>
+      </c>
+      <c r="L26" s="11">
+        <f t="shared" si="10"/>
+        <v>0.15875</v>
+      </c>
+      <c r="M26" s="18"/>
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="18">
+        <v>1</v>
+      </c>
+      <c r="H27" s="14">
+        <v>8.81</v>
+      </c>
+      <c r="I27" s="14">
+        <f>G27*H27</f>
+        <v>8.81</v>
+      </c>
+      <c r="J27" s="19">
+        <v>25</v>
+      </c>
+      <c r="K27" s="11">
+        <f>IF(G27&gt;0,(J27/1000)*G27*H27,0)</f>
         <v>0.22025000000000003</v>
       </c>
-      <c r="L25" s="11">
-        <f t="shared" si="9"/>
+      <c r="L27" s="11">
+        <f>K27</f>
         <v>0.22025000000000003</v>
       </c>
-      <c r="M25" s="18"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64"/>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
-      <c r="X25" s="64"/>
-      <c r="Y25" s="64"/>
-      <c r="Z25" s="64"/>
-      <c r="AA25" s="64"/>
-      <c r="AB25" s="64"/>
-      <c r="AC25" s="64"/>
-      <c r="AD25" s="64"/>
-      <c r="AE25" s="64"/>
-      <c r="AF25" s="64"/>
-      <c r="AG25" s="64"/>
-      <c r="AH25" s="64"/>
-      <c r="AI25" s="64"/>
-      <c r="AJ25" s="64"/>
-    </row>
-    <row r="26" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-    </row>
-    <row r="27" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="39" t="s">
+      <c r="M27" s="18"/>
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="14"/>
+    </row>
+    <row r="29" spans="1:48" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="14">
+        <v>1</v>
+      </c>
+      <c r="H29" s="14">
+        <v>4.87</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" ref="I29" si="11">G29*H29</f>
+        <v>4.87</v>
+      </c>
+      <c r="J29" s="19">
+        <v>25</v>
+      </c>
+      <c r="K29" s="11">
+        <f>IF(G29&gt;0,(J29/1000)*G29*H29,0)</f>
+        <v>0.12175000000000001</v>
+      </c>
+      <c r="L29" s="11">
+        <f t="shared" ref="L29" si="12">K29</f>
+        <v>0.12175000000000001</v>
+      </c>
+      <c r="M29" s="18"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+    </row>
+    <row r="30" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="53"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
+    </row>
+    <row r="31" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
+      <c r="B31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="31"/>
-    </row>
-    <row r="28" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="50" t="s">
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="31"/>
+    </row>
+    <row r="32" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
+      <c r="B32" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C32" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="50" t="s">
+      <c r="D32" s="21"/>
+      <c r="E32" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F32" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="50" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B34" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B35" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-    </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
-      <c r="B35" s="40" t="s">
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="34"/>
+      <c r="B39" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="52"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="12" t="s">
+      <c r="C39" s="35"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="52"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="36"/>
+      <c r="B40" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12" t="s">
+      <c r="D40" s="12"/>
+      <c r="E40" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G40" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H40" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I40" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="J40" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K40" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="L40" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="22">
+        <v>1</v>
+      </c>
+      <c r="H41" s="22">
+        <v>1</v>
+      </c>
+      <c r="I41" s="22">
+        <f t="shared" ref="I41" si="13">IF(G41&gt;0,CEILING(G41/H41,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="22">
+        <v>83.65</v>
+      </c>
+      <c r="K41" s="22">
+        <f>IF(G41&gt;0,J41/H41*G41,0)</f>
+        <v>83.65</v>
+      </c>
+      <c r="L41" s="22">
+        <f t="shared" ref="L41" si="14">I41*J41</f>
+        <v>83.65</v>
+      </c>
+      <c r="M41" s="22"/>
+      <c r="N41" s="70" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="A21:N21"/>
+    <mergeCell ref="A23:N23"/>
     <mergeCell ref="A12:N12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2298,13 +2508,24 @@
     <hyperlink ref="N10" r:id="rId2" xr:uid="{EE7378BE-0B25-416E-BEFF-DB538344FEE5}"/>
     <hyperlink ref="N11" r:id="rId3" xr:uid="{FCFB70A5-1843-4D95-9CBC-02997102CAEA}"/>
     <hyperlink ref="N14" r:id="rId4" xr:uid="{BD7999A7-5D30-4B03-A052-3FA1F4EC70A1}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{5CAAD5F5-20A3-41A9-AA2D-BB80E4ED617D}"/>
+    <hyperlink ref="N41" r:id="rId6" xr:uid="{C195FD31-3949-4366-959B-35D6ED3143B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
@@ -2313,15 +2534,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2574,20 +2786,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
     <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>